<commit_message>
add viewers annotations to the emfxcel example
</commit_message>
<xml_diff>
--- a/emfxcel/net.istvanrath.emfxcel.incquery/samples/studentscourses.xlsx
+++ b/emfxcel/net.istvanrath.emfxcel.incquery/samples/studentscourses.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-35660" yWindow="0" windowWidth="16960" windowHeight="20400" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="9200" windowHeight="13920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>First name</t>
   </si>
@@ -52,62 +52,62 @@
     <t>Horváth</t>
   </si>
   <si>
+    <t>Bergmann</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>UZ0</t>
+  </si>
+  <si>
+    <t>AH1</t>
+  </si>
+  <si>
+    <t>IR2</t>
+  </si>
+  <si>
+    <t>AH2</t>
+  </si>
+  <si>
+    <t>GB3</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>Student Identifier</t>
+  </si>
+  <si>
+    <t>Formal methods</t>
+  </si>
+  <si>
+    <t>András Pataricza</t>
+  </si>
+  <si>
+    <t>Model-driven software engineering</t>
+  </si>
+  <si>
+    <t>Dániel Varró</t>
+  </si>
+  <si>
+    <t>Eclipse programming</t>
+  </si>
+  <si>
+    <t>István Majzik</t>
+  </si>
+  <si>
     <t>Gábor</t>
-  </si>
-  <si>
-    <t>Bergmann</t>
-  </si>
-  <si>
-    <t>Course</t>
-  </si>
-  <si>
-    <t>Identifier</t>
-  </si>
-  <si>
-    <t>UZ0</t>
-  </si>
-  <si>
-    <t>AH1</t>
-  </si>
-  <si>
-    <t>IR2</t>
-  </si>
-  <si>
-    <t>AH2</t>
-  </si>
-  <si>
-    <t>GB3</t>
-  </si>
-  <si>
-    <t>Teacher</t>
-  </si>
-  <si>
-    <t>Student Identifier</t>
-  </si>
-  <si>
-    <t>Formal methods</t>
-  </si>
-  <si>
-    <t>András Pataricza</t>
-  </si>
-  <si>
-    <t>Model-driven software engineering</t>
-  </si>
-  <si>
-    <t>Dániel Varró</t>
-  </si>
-  <si>
-    <t>Eclipse programming</t>
-  </si>
-  <si>
-    <t>István Majzik</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -122,6 +122,24 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -142,14 +160,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -482,7 +504,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -495,7 +517,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -506,7 +528,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -517,7 +539,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -528,7 +550,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -539,18 +561,18 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -565,10 +587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -580,83 +602,95 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>